<commit_message>
computed for year and car age
</commit_message>
<xml_diff>
--- a/excel/car_database/car database.xlsx
+++ b/excel/car_database/car database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\mikedevs\data-journey\excel\car_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F342E470-17D7-4D76-B73D-9895C20561D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B276EA-995A-431F-96E7-7F7571F4719B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{196D0D68-09E0-4E97-9B35-E2D7744763AB}"/>
   </bookViews>
@@ -100,9 +100,6 @@
     <t>FD08MTG005</t>
   </si>
   <si>
-    <t>FDO6FCS006</t>
-  </si>
-  <si>
     <t>Ewenty</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>Rodriguez</t>
   </si>
   <si>
-    <t>GMO9CMR014</t>
-  </si>
-  <si>
     <t>Santos</t>
   </si>
   <si>
@@ -238,9 +232,6 @@
     <t>HO13CIV036</t>
   </si>
   <si>
-    <t>HOO5ODY037</t>
-  </si>
-  <si>
     <t>HO07ODY038</t>
   </si>
   <si>
@@ -386,6 +377,15 @@
   </si>
   <si>
     <t>HO01ODY040</t>
+  </si>
+  <si>
+    <t>FD06FCS006</t>
+  </si>
+  <si>
+    <t>GM09CMR014</t>
+  </si>
+  <si>
+    <t>HO05ODY037</t>
   </si>
 </sst>
 </file>
@@ -1228,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF49C490-40C4-41A8-88BF-87A5D58F4AC8}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1305,6 +1305,14 @@
         <f>VLOOKUP(D2,D$56:E$66,2)</f>
         <v>Mustang</v>
       </c>
+      <c r="F2" t="str">
+        <f>MID(A2,3,2)</f>
+        <v>06</v>
+      </c>
+      <c r="G2">
+        <f>IF(25-F2&lt;0,100-F2+25,25-F2)</f>
+        <v>19</v>
+      </c>
       <c r="H2">
         <v>40326.800000000003</v>
       </c>
@@ -1338,6 +1346,14 @@
         <f t="shared" ref="E3:E53" si="3">VLOOKUP(D3,D$56:E$66,2)</f>
         <v>Mustang</v>
       </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F53" si="4">MID(A3,3,2)</f>
+        <v>06</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G53" si="5">IF(25-F3&lt;0,100-F3+25,25-F3)</f>
+        <v>19</v>
+      </c>
       <c r="H3">
         <v>44974.8</v>
       </c>
@@ -1371,6 +1387,14 @@
         <f t="shared" si="3"/>
         <v>Mustang</v>
       </c>
+      <c r="F4" t="str">
+        <f t="shared" si="4"/>
+        <v>08</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
       <c r="H4">
         <v>44946.5</v>
       </c>
@@ -1404,6 +1428,14 @@
         <f t="shared" si="3"/>
         <v>Mustang</v>
       </c>
+      <c r="F5" t="str">
+        <f t="shared" si="4"/>
+        <v>08</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
       <c r="H5">
         <v>37558.800000000003</v>
       </c>
@@ -1437,6 +1469,14 @@
         <f t="shared" si="3"/>
         <v>Mustang</v>
       </c>
+      <c r="F6" t="str">
+        <f t="shared" si="4"/>
+        <v>08</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
       <c r="H6">
         <v>36438.5</v>
       </c>
@@ -1452,7 +1492,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -1469,6 +1509,14 @@
       <c r="E7" t="str">
         <f t="shared" si="3"/>
         <v>Focus</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="4"/>
+        <v>06</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="5"/>
+        <v>19</v>
       </c>
       <c r="H7">
         <v>46311.4</v>
@@ -1477,7 +1525,7 @@
         <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7">
         <v>75000</v>
@@ -1485,7 +1533,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -1502,6 +1550,14 @@
       <c r="E8" t="str">
         <f t="shared" si="3"/>
         <v>Focus</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="4"/>
+        <v>06</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="5"/>
+        <v>19</v>
       </c>
       <c r="H8">
         <v>52229.5</v>
@@ -1518,7 +1574,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -1535,6 +1591,14 @@
       <c r="E9" t="str">
         <f t="shared" si="3"/>
         <v>Focus</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="4"/>
+        <v>09</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="H9">
         <v>35137</v>
@@ -1543,7 +1607,7 @@
         <v>15</v>
       </c>
       <c r="K9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L9">
         <v>75000</v>
@@ -1551,7 +1615,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -1568,6 +1632,14 @@
       <c r="E10" t="str">
         <f t="shared" si="3"/>
         <v>Focus</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="H10">
         <v>27637.1</v>
@@ -1584,7 +1656,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -1601,6 +1673,14 @@
       <c r="E11" t="str">
         <f t="shared" si="3"/>
         <v>Focus</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="H11">
         <v>27534.799999999999</v>
@@ -1609,7 +1689,7 @@
         <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L11">
         <v>75000</v>
@@ -1617,7 +1697,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -1634,6 +1714,14 @@
       <c r="E12" t="str">
         <f t="shared" si="3"/>
         <v>Focus</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="H12">
         <v>19341.7</v>
@@ -1642,7 +1730,7 @@
         <v>18</v>
       </c>
       <c r="K12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L12">
         <v>75000</v>
@@ -1650,7 +1738,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -1667,6 +1755,14 @@
       <c r="E13" t="str">
         <f t="shared" si="3"/>
         <v>Focus</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="H13">
         <v>22521.599999999999</v>
@@ -1675,7 +1771,7 @@
         <v>15</v>
       </c>
       <c r="K13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L13">
         <v>75000</v>
@@ -1683,7 +1779,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -1701,6 +1797,14 @@
         <f t="shared" si="3"/>
         <v>Focus</v>
       </c>
+      <c r="F14" t="str">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
       <c r="H14">
         <v>13682.9</v>
       </c>
@@ -1708,7 +1812,7 @@
         <v>15</v>
       </c>
       <c r="K14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L14">
         <v>75000</v>
@@ -1716,7 +1820,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -1733,6 +1837,14 @@
       <c r="E15" t="str">
         <f t="shared" si="3"/>
         <v>Camero</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="4"/>
+        <v>09</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="H15">
         <v>28464.799999999999</v>
@@ -1741,7 +1853,7 @@
         <v>18</v>
       </c>
       <c r="K15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L15">
         <v>100000</v>
@@ -1749,7 +1861,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -1766,6 +1878,14 @@
       <c r="E16" t="str">
         <f t="shared" si="3"/>
         <v>Camero</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="H16">
         <v>19421.099999999999</v>
@@ -1774,7 +1894,7 @@
         <v>15</v>
       </c>
       <c r="K16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L16">
         <v>100000</v>
@@ -1782,7 +1902,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -1799,6 +1919,14 @@
       <c r="E17" t="str">
         <f t="shared" si="3"/>
         <v>Camero</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="H17">
         <v>14289.6</v>
@@ -1807,7 +1935,7 @@
         <v>18</v>
       </c>
       <c r="K17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L17">
         <v>100000</v>
@@ -1815,7 +1943,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -1832,6 +1960,14 @@
       <c r="E18" t="str">
         <f t="shared" si="3"/>
         <v>Silverado</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>15</v>
       </c>
       <c r="H18">
         <v>31144.400000000001</v>
@@ -1840,7 +1976,7 @@
         <v>15</v>
       </c>
       <c r="K18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L18">
         <v>100000</v>
@@ -1848,7 +1984,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -1865,6 +2001,14 @@
       <c r="E19" t="str">
         <f t="shared" si="3"/>
         <v>Silverado</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>27</v>
       </c>
       <c r="H19">
         <v>83162.7</v>
@@ -1873,7 +2017,7 @@
         <v>15</v>
       </c>
       <c r="K19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L19">
         <v>100000</v>
@@ -1881,7 +2025,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -1898,15 +2042,23 @@
       <c r="E20" t="str">
         <f t="shared" si="3"/>
         <v>Silverado</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="4"/>
+        <v>00</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>25</v>
       </c>
       <c r="H20">
         <v>80685.8</v>
       </c>
       <c r="J20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L20">
         <v>100000</v>
@@ -1914,7 +2066,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
@@ -1931,6 +2083,14 @@
       <c r="E21" t="str">
         <f t="shared" si="3"/>
         <v>Camry</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>29</v>
       </c>
       <c r="H21">
         <v>114660.6</v>
@@ -1939,7 +2099,7 @@
         <v>21</v>
       </c>
       <c r="K21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L21">
         <v>100000</v>
@@ -1947,7 +2107,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -1964,6 +2124,14 @@
       <c r="E22" t="str">
         <f t="shared" si="3"/>
         <v>Camry</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>27</v>
       </c>
       <c r="H22">
         <v>93382.6</v>
@@ -1972,7 +2140,7 @@
         <v>15</v>
       </c>
       <c r="K22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L22">
         <v>100000</v>
@@ -1980,7 +2148,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -1997,6 +2165,14 @@
       <c r="E23" t="str">
         <f t="shared" si="3"/>
         <v>Camry</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="4"/>
+        <v>00</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>25</v>
       </c>
       <c r="H23">
         <v>85928</v>
@@ -2005,7 +2181,7 @@
         <v>21</v>
       </c>
       <c r="K23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L23">
         <v>100000</v>
@@ -2013,7 +2189,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -2030,6 +2206,14 @@
       <c r="E24" t="str">
         <f t="shared" si="3"/>
         <v>Camry</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="4"/>
+        <v>02</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>23</v>
       </c>
       <c r="H24">
         <v>67829.100000000006</v>
@@ -2046,7 +2230,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -2063,6 +2247,14 @@
       <c r="E25" t="str">
         <f t="shared" si="3"/>
         <v>Camry</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="4"/>
+        <v>09</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="H25">
         <v>48114.2</v>
@@ -2071,7 +2263,7 @@
         <v>18</v>
       </c>
       <c r="K25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L25">
         <v>100000</v>
@@ -2079,7 +2271,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -2096,15 +2288,23 @@
       <c r="E26" t="str">
         <f t="shared" si="3"/>
         <v>Corolla</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="4"/>
+        <v>02</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>23</v>
       </c>
       <c r="H26">
         <v>64467.4</v>
       </c>
       <c r="J26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L26">
         <v>100000</v>
@@ -2112,7 +2312,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
@@ -2129,6 +2329,14 @@
       <c r="E27" t="str">
         <f t="shared" si="3"/>
         <v>Corolla</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="4"/>
+        <v>03</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>22</v>
       </c>
       <c r="H27">
         <v>73444.399999999994</v>
@@ -2137,7 +2345,7 @@
         <v>15</v>
       </c>
       <c r="K27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L27">
         <v>100000</v>
@@ -2145,7 +2353,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
@@ -2162,15 +2370,23 @@
       <c r="E28" t="str">
         <f t="shared" si="3"/>
         <v>Corolla</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="H28">
         <v>17556.3</v>
       </c>
       <c r="J28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L28">
         <v>100000</v>
@@ -2178,7 +2394,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
@@ -2195,6 +2411,14 @@
       <c r="E29" t="str">
         <f t="shared" si="3"/>
         <v>Corolla</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="H29">
         <v>29601.9</v>
@@ -2203,7 +2427,7 @@
         <v>15</v>
       </c>
       <c r="K29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L29">
         <v>100000</v>
@@ -2211,7 +2435,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -2228,15 +2452,23 @@
       <c r="E30" t="str">
         <f t="shared" si="3"/>
         <v>Camry</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="H30">
         <v>22128.2</v>
       </c>
       <c r="J30" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" t="s">
         <v>50</v>
-      </c>
-      <c r="K30" t="s">
-        <v>52</v>
       </c>
       <c r="L30">
         <v>100000</v>
@@ -2244,7 +2476,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -2261,6 +2493,14 @@
       <c r="E31" t="str">
         <f t="shared" si="3"/>
         <v>Civic</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>26</v>
       </c>
       <c r="H31">
         <v>82374</v>
@@ -2269,7 +2509,7 @@
         <v>18</v>
       </c>
       <c r="K31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L31">
         <v>75000</v>
@@ -2277,7 +2517,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -2294,12 +2534,20 @@
       <c r="E32" t="str">
         <f t="shared" si="3"/>
         <v>Civic</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="4"/>
+        <v>01</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>24</v>
       </c>
       <c r="H32">
         <v>69891.899999999994</v>
       </c>
       <c r="J32" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K32" t="s">
         <v>24</v>
@@ -2310,7 +2558,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
@@ -2327,15 +2575,23 @@
       <c r="E33" t="str">
         <f t="shared" si="3"/>
         <v>Civic</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="5"/>
+        <v>15</v>
       </c>
       <c r="H33">
         <v>22573</v>
       </c>
       <c r="J33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L33">
         <v>75000</v>
@@ -2343,7 +2599,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
@@ -2360,6 +2616,14 @@
       <c r="E34" t="str">
         <f t="shared" si="3"/>
         <v>Civic</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="5"/>
+        <v>15</v>
       </c>
       <c r="H34">
         <v>33477.199999999997</v>
@@ -2368,7 +2632,7 @@
         <v>15</v>
       </c>
       <c r="K34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L34">
         <v>75000</v>
@@ -2376,7 +2640,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
@@ -2393,6 +2657,14 @@
       <c r="E35" t="str">
         <f t="shared" si="3"/>
         <v>Civic</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="H35">
         <v>30555.3</v>
@@ -2409,7 +2681,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
@@ -2426,6 +2698,14 @@
       <c r="E36" t="str">
         <f t="shared" si="3"/>
         <v>Civic</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="H36">
         <v>24513.200000000001</v>
@@ -2434,7 +2714,7 @@
         <v>15</v>
       </c>
       <c r="K36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L36">
         <v>75000</v>
@@ -2442,7 +2722,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
@@ -2459,6 +2739,14 @@
       <c r="E37" t="str">
         <f t="shared" si="3"/>
         <v>Civic</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="H37">
         <v>13867.6</v>
@@ -2467,7 +2755,7 @@
         <v>15</v>
       </c>
       <c r="K37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L37">
         <v>75000</v>
@@ -2475,7 +2763,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
@@ -2492,6 +2780,14 @@
       <c r="E38" t="str">
         <f t="shared" si="3"/>
         <v>Odyssy</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="4"/>
+        <v>05</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="5"/>
+        <v>20</v>
       </c>
       <c r="H38">
         <v>60389.5</v>
@@ -2500,7 +2796,7 @@
         <v>18</v>
       </c>
       <c r="K38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L38">
         <v>100000</v>
@@ -2508,7 +2804,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
@@ -2525,6 +2821,14 @@
       <c r="E39" t="str">
         <f t="shared" si="3"/>
         <v>Odyssy</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="4"/>
+        <v>07</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="H39">
         <v>50854.1</v>
@@ -2533,7 +2837,7 @@
         <v>15</v>
       </c>
       <c r="K39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L39">
         <v>100000</v>
@@ -2541,7 +2845,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
@@ -2558,6 +2862,14 @@
       <c r="E40" t="str">
         <f t="shared" si="3"/>
         <v>Odyssy</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="4"/>
+        <v>08</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
       <c r="H40">
         <v>42504.6</v>
@@ -2566,7 +2878,7 @@
         <v>18</v>
       </c>
       <c r="K40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L40">
         <v>100000</v>
@@ -2574,7 +2886,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
@@ -2592,6 +2904,14 @@
         <f t="shared" si="3"/>
         <v>Odyssy</v>
       </c>
+      <c r="F41" t="str">
+        <f t="shared" si="4"/>
+        <v>01</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
       <c r="H41">
         <v>68658.899999999994</v>
       </c>
@@ -2607,7 +2927,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
@@ -2624,6 +2944,14 @@
       <c r="E42" t="str">
         <f t="shared" si="3"/>
         <v>Odyssy</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="H42">
         <v>3708.1</v>
@@ -2640,7 +2968,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
@@ -2657,12 +2985,20 @@
       <c r="E43" t="str">
         <f t="shared" si="3"/>
         <v>PT Cruiser</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="4"/>
+        <v>04</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="5"/>
+        <v>21</v>
       </c>
       <c r="H43">
         <v>64542</v>
       </c>
       <c r="J43" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K43" t="s">
         <v>16</v>
@@ -2673,7 +3009,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
@@ -2690,6 +3026,14 @@
       <c r="E44" t="str">
         <f t="shared" si="3"/>
         <v>PT Cruiser</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="4"/>
+        <v>07</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="H44">
         <v>42074.2</v>
@@ -2698,7 +3042,7 @@
         <v>21</v>
       </c>
       <c r="K44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L44">
         <v>75000</v>
@@ -2706,7 +3050,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
@@ -2723,6 +3067,14 @@
       <c r="E45" t="str">
         <f t="shared" si="3"/>
         <v>PT Cruiser</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="H45">
         <v>27394.2</v>
@@ -2731,7 +3083,7 @@
         <v>15</v>
       </c>
       <c r="K45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L45">
         <v>75000</v>
@@ -2739,7 +3091,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
@@ -2756,6 +3108,14 @@
       <c r="E46" t="str">
         <f t="shared" si="3"/>
         <v>Caravan</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="5"/>
+        <v>26</v>
       </c>
       <c r="H46">
         <v>79420.600000000006</v>
@@ -2764,7 +3124,7 @@
         <v>21</v>
       </c>
       <c r="K46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L46">
         <v>75000</v>
@@ -2772,7 +3132,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
@@ -2789,6 +3149,14 @@
       <c r="E47" t="str">
         <f t="shared" si="3"/>
         <v>Caravan</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="4"/>
+        <v>00</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="5"/>
+        <v>25</v>
       </c>
       <c r="H47">
         <v>77243.100000000006</v>
@@ -2805,7 +3173,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
@@ -2822,6 +3190,14 @@
       <c r="E48" t="str">
         <f t="shared" si="3"/>
         <v>Caravan</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="4"/>
+        <v>04</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="5"/>
+        <v>21</v>
       </c>
       <c r="H48">
         <v>72527.199999999997</v>
@@ -2830,7 +3206,7 @@
         <v>18</v>
       </c>
       <c r="K48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L48">
         <v>75000</v>
@@ -2838,7 +3214,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
@@ -2855,15 +3231,23 @@
       <c r="E49" t="str">
         <f t="shared" si="3"/>
         <v>Caravan</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="4"/>
+        <v>04</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="5"/>
+        <v>21</v>
       </c>
       <c r="H49">
         <v>52699.4</v>
       </c>
       <c r="J49" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K49" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L49">
         <v>75000</v>
@@ -2871,7 +3255,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
@@ -2888,6 +3272,14 @@
       <c r="E50" t="str">
         <f t="shared" si="3"/>
         <v>Elantra</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="H50">
         <v>29102.3</v>
@@ -2896,7 +3288,7 @@
         <v>15</v>
       </c>
       <c r="K50" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L50">
         <v>100000</v>
@@ -2904,7 +3296,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
@@ -2921,12 +3313,20 @@
       <c r="E51" t="str">
         <f t="shared" si="3"/>
         <v>Elantra</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="H51">
         <v>22282</v>
       </c>
       <c r="J51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K51" t="s">
         <v>19</v>
@@ -2937,7 +3337,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
@@ -2954,6 +3354,14 @@
       <c r="E52" t="str">
         <f t="shared" si="3"/>
         <v>Elantra</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="H52">
         <v>20223.900000000001</v>
@@ -2962,7 +3370,7 @@
         <v>15</v>
       </c>
       <c r="K52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L52">
         <v>100000</v>
@@ -2970,7 +3378,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
@@ -2987,15 +3395,23 @@
       <c r="E53" t="str">
         <f t="shared" si="3"/>
         <v>Elantra</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="H53">
         <v>22188.5</v>
       </c>
       <c r="J53" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L53">
         <v>100000</v>
@@ -3003,126 +3419,126 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D56" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E56" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C57" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D57" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E57" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C58" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D58" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E58" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D59" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E59" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C60" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D60" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E60" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D61" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E61" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D62" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E62" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D63" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E63" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D64" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E64" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D65" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D66" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E66" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
computed for miles per year
</commit_message>
<xml_diff>
--- a/excel/car_database/car database.xlsx
+++ b/excel/car_database/car database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\mikedevs\data-journey\excel\car_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B276EA-995A-431F-96E7-7F7571F4719B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4924FA7D-2C83-4092-BD94-9125C30DC026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{196D0D68-09E0-4E97-9B35-E2D7744763AB}"/>
   </bookViews>
@@ -1229,7 +1229,7 @@
   <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1316,6 +1316,10 @@
       <c r="H2">
         <v>40326.800000000003</v>
       </c>
+      <c r="I2">
+        <f>H2/G2</f>
+        <v>2122.4631578947369</v>
+      </c>
       <c r="J2" t="s">
         <v>15</v>
       </c>
@@ -1357,6 +1361,10 @@
       <c r="H3">
         <v>44974.8</v>
       </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I53" si="6">H3/G3</f>
+        <v>2367.0947368421052</v>
+      </c>
       <c r="J3" t="s">
         <v>18</v>
       </c>
@@ -1398,6 +1406,10 @@
       <c r="H4">
         <v>44946.5</v>
       </c>
+      <c r="I4">
+        <f t="shared" si="6"/>
+        <v>2643.9117647058824</v>
+      </c>
       <c r="J4" t="s">
         <v>21</v>
       </c>
@@ -1439,6 +1451,10 @@
       <c r="H5">
         <v>37558.800000000003</v>
       </c>
+      <c r="I5">
+        <f t="shared" si="6"/>
+        <v>2209.3411764705884</v>
+      </c>
       <c r="J5" t="s">
         <v>15</v>
       </c>
@@ -1480,6 +1496,10 @@
       <c r="H6">
         <v>36438.5</v>
       </c>
+      <c r="I6">
+        <f t="shared" si="6"/>
+        <v>2143.4411764705883</v>
+      </c>
       <c r="J6" t="s">
         <v>18</v>
       </c>
@@ -1521,6 +1541,10 @@
       <c r="H7">
         <v>46311.4</v>
       </c>
+      <c r="I7">
+        <f t="shared" si="6"/>
+        <v>2437.4421052631578</v>
+      </c>
       <c r="J7" t="s">
         <v>21</v>
       </c>
@@ -1562,6 +1586,10 @@
       <c r="H8">
         <v>52229.5</v>
       </c>
+      <c r="I8">
+        <f t="shared" si="6"/>
+        <v>2748.9210526315787</v>
+      </c>
       <c r="J8" t="s">
         <v>21</v>
       </c>
@@ -1603,6 +1631,10 @@
       <c r="H9">
         <v>35137</v>
       </c>
+      <c r="I9">
+        <f t="shared" si="6"/>
+        <v>2196.0625</v>
+      </c>
       <c r="J9" t="s">
         <v>15</v>
       </c>
@@ -1644,6 +1676,10 @@
       <c r="H10">
         <v>27637.1</v>
       </c>
+      <c r="I10">
+        <f t="shared" si="6"/>
+        <v>2303.0916666666667</v>
+      </c>
       <c r="J10" t="s">
         <v>15</v>
       </c>
@@ -1685,6 +1721,10 @@
       <c r="H11">
         <v>27534.799999999999</v>
       </c>
+      <c r="I11">
+        <f t="shared" si="6"/>
+        <v>2294.5666666666666</v>
+      </c>
       <c r="J11" t="s">
         <v>18</v>
       </c>
@@ -1726,6 +1766,10 @@
       <c r="H12">
         <v>19341.7</v>
       </c>
+      <c r="I12">
+        <f t="shared" si="6"/>
+        <v>1487.823076923077</v>
+      </c>
       <c r="J12" t="s">
         <v>18</v>
       </c>
@@ -1767,6 +1811,10 @@
       <c r="H13">
         <v>22521.599999999999</v>
       </c>
+      <c r="I13">
+        <f t="shared" si="6"/>
+        <v>1876.8</v>
+      </c>
       <c r="J13" t="s">
         <v>15</v>
       </c>
@@ -1808,6 +1856,10 @@
       <c r="H14">
         <v>13682.9</v>
       </c>
+      <c r="I14">
+        <f t="shared" si="6"/>
+        <v>1140.2416666666666</v>
+      </c>
       <c r="J14" t="s">
         <v>15</v>
       </c>
@@ -1849,6 +1901,10 @@
       <c r="H15">
         <v>28464.799999999999</v>
       </c>
+      <c r="I15">
+        <f t="shared" si="6"/>
+        <v>1779.05</v>
+      </c>
       <c r="J15" t="s">
         <v>18</v>
       </c>
@@ -1890,6 +1946,10 @@
       <c r="H16">
         <v>19421.099999999999</v>
       </c>
+      <c r="I16">
+        <f t="shared" si="6"/>
+        <v>1493.9307692307691</v>
+      </c>
       <c r="J16" t="s">
         <v>15</v>
       </c>
@@ -1931,6 +1991,10 @@
       <c r="H17">
         <v>14289.6</v>
       </c>
+      <c r="I17">
+        <f t="shared" si="6"/>
+        <v>1299.0545454545454</v>
+      </c>
       <c r="J17" t="s">
         <v>18</v>
       </c>
@@ -1972,6 +2036,10 @@
       <c r="H18">
         <v>31144.400000000001</v>
       </c>
+      <c r="I18">
+        <f t="shared" si="6"/>
+        <v>2076.2933333333335</v>
+      </c>
       <c r="J18" t="s">
         <v>15</v>
       </c>
@@ -2013,6 +2081,10 @@
       <c r="H19">
         <v>83162.7</v>
       </c>
+      <c r="I19">
+        <f t="shared" si="6"/>
+        <v>3080.1</v>
+      </c>
       <c r="J19" t="s">
         <v>15</v>
       </c>
@@ -2054,6 +2126,10 @@
       <c r="H20">
         <v>80685.8</v>
       </c>
+      <c r="I20">
+        <f t="shared" si="6"/>
+        <v>3227.4320000000002</v>
+      </c>
       <c r="J20" t="s">
         <v>48</v>
       </c>
@@ -2095,6 +2171,10 @@
       <c r="H21">
         <v>114660.6</v>
       </c>
+      <c r="I21">
+        <f t="shared" si="6"/>
+        <v>3953.8137931034485</v>
+      </c>
       <c r="J21" t="s">
         <v>21</v>
       </c>
@@ -2136,6 +2216,10 @@
       <c r="H22">
         <v>93382.6</v>
       </c>
+      <c r="I22">
+        <f t="shared" si="6"/>
+        <v>3458.614814814815</v>
+      </c>
       <c r="J22" t="s">
         <v>15</v>
       </c>
@@ -2177,6 +2261,10 @@
       <c r="H23">
         <v>85928</v>
       </c>
+      <c r="I23">
+        <f t="shared" si="6"/>
+        <v>3437.12</v>
+      </c>
       <c r="J23" t="s">
         <v>21</v>
       </c>
@@ -2218,6 +2306,10 @@
       <c r="H24">
         <v>67829.100000000006</v>
       </c>
+      <c r="I24">
+        <f t="shared" si="6"/>
+        <v>2949.0913043478263</v>
+      </c>
       <c r="J24" t="s">
         <v>15</v>
       </c>
@@ -2259,6 +2351,10 @@
       <c r="H25">
         <v>48114.2</v>
       </c>
+      <c r="I25">
+        <f t="shared" si="6"/>
+        <v>3007.1374999999998</v>
+      </c>
       <c r="J25" t="s">
         <v>18</v>
       </c>
@@ -2300,6 +2396,10 @@
       <c r="H26">
         <v>64467.4</v>
       </c>
+      <c r="I26">
+        <f t="shared" si="6"/>
+        <v>2802.9304347826087</v>
+      </c>
       <c r="J26" t="s">
         <v>57</v>
       </c>
@@ -2341,6 +2441,10 @@
       <c r="H27">
         <v>73444.399999999994</v>
       </c>
+      <c r="I27">
+        <f t="shared" si="6"/>
+        <v>3338.3818181818178</v>
+      </c>
       <c r="J27" t="s">
         <v>15</v>
       </c>
@@ -2382,6 +2486,10 @@
       <c r="H28">
         <v>17556.3</v>
       </c>
+      <c r="I28">
+        <f t="shared" si="6"/>
+        <v>1596.0272727272727</v>
+      </c>
       <c r="J28" t="s">
         <v>48</v>
       </c>
@@ -2423,6 +2531,10 @@
       <c r="H29">
         <v>29601.9</v>
       </c>
+      <c r="I29">
+        <f t="shared" si="6"/>
+        <v>2277.0692307692307</v>
+      </c>
       <c r="J29" t="s">
         <v>15</v>
       </c>
@@ -2464,6 +2576,10 @@
       <c r="H30">
         <v>22128.2</v>
       </c>
+      <c r="I30">
+        <f t="shared" si="6"/>
+        <v>1702.1692307692308</v>
+      </c>
       <c r="J30" t="s">
         <v>48</v>
       </c>
@@ -2505,6 +2621,10 @@
       <c r="H31">
         <v>82374</v>
       </c>
+      <c r="I31">
+        <f t="shared" si="6"/>
+        <v>3168.2307692307691</v>
+      </c>
       <c r="J31" t="s">
         <v>18</v>
       </c>
@@ -2546,6 +2666,10 @@
       <c r="H32">
         <v>69891.899999999994</v>
       </c>
+      <c r="I32">
+        <f t="shared" si="6"/>
+        <v>2912.1624999999999</v>
+      </c>
       <c r="J32" t="s">
         <v>48</v>
       </c>
@@ -2587,6 +2711,10 @@
       <c r="H33">
         <v>22573</v>
       </c>
+      <c r="I33">
+        <f t="shared" si="6"/>
+        <v>1504.8666666666666</v>
+      </c>
       <c r="J33" t="s">
         <v>48</v>
       </c>
@@ -2628,6 +2756,10 @@
       <c r="H34">
         <v>33477.199999999997</v>
       </c>
+      <c r="I34">
+        <f t="shared" si="6"/>
+        <v>2231.813333333333</v>
+      </c>
       <c r="J34" t="s">
         <v>15</v>
       </c>
@@ -2669,6 +2801,10 @@
       <c r="H35">
         <v>30555.3</v>
       </c>
+      <c r="I35">
+        <f t="shared" si="6"/>
+        <v>2182.5214285714287</v>
+      </c>
       <c r="J35" t="s">
         <v>15</v>
       </c>
@@ -2710,6 +2846,10 @@
       <c r="H36">
         <v>24513.200000000001</v>
       </c>
+      <c r="I36">
+        <f t="shared" si="6"/>
+        <v>1885.6307692307694</v>
+      </c>
       <c r="J36" t="s">
         <v>15</v>
       </c>
@@ -2751,6 +2891,10 @@
       <c r="H37">
         <v>13867.6</v>
       </c>
+      <c r="I37">
+        <f t="shared" si="6"/>
+        <v>1155.6333333333334</v>
+      </c>
       <c r="J37" t="s">
         <v>15</v>
       </c>
@@ -2792,6 +2936,10 @@
       <c r="H38">
         <v>60389.5</v>
       </c>
+      <c r="I38">
+        <f t="shared" si="6"/>
+        <v>3019.4749999999999</v>
+      </c>
       <c r="J38" t="s">
         <v>18</v>
       </c>
@@ -2833,6 +2981,10 @@
       <c r="H39">
         <v>50854.1</v>
       </c>
+      <c r="I39">
+        <f t="shared" si="6"/>
+        <v>2825.2277777777776</v>
+      </c>
       <c r="J39" t="s">
         <v>15</v>
       </c>
@@ -2874,6 +3026,10 @@
       <c r="H40">
         <v>42504.6</v>
       </c>
+      <c r="I40">
+        <f t="shared" si="6"/>
+        <v>2500.2705882352939</v>
+      </c>
       <c r="J40" t="s">
         <v>18</v>
       </c>
@@ -2915,6 +3071,10 @@
       <c r="H41">
         <v>68658.899999999994</v>
       </c>
+      <c r="I41">
+        <f t="shared" si="6"/>
+        <v>2860.7874999999999</v>
+      </c>
       <c r="J41" t="s">
         <v>15</v>
       </c>
@@ -2956,6 +3116,10 @@
       <c r="H42">
         <v>3708.1</v>
       </c>
+      <c r="I42">
+        <f t="shared" si="6"/>
+        <v>337.09999999999997</v>
+      </c>
       <c r="J42" t="s">
         <v>15</v>
       </c>
@@ -2997,6 +3161,10 @@
       <c r="H43">
         <v>64542</v>
       </c>
+      <c r="I43">
+        <f t="shared" si="6"/>
+        <v>3073.4285714285716</v>
+      </c>
       <c r="J43" t="s">
         <v>48</v>
       </c>
@@ -3038,6 +3206,10 @@
       <c r="H44">
         <v>42074.2</v>
       </c>
+      <c r="I44">
+        <f t="shared" si="6"/>
+        <v>2337.4555555555553</v>
+      </c>
       <c r="J44" t="s">
         <v>21</v>
       </c>
@@ -3079,6 +3251,10 @@
       <c r="H45">
         <v>27394.2</v>
       </c>
+      <c r="I45">
+        <f t="shared" si="6"/>
+        <v>1956.7285714285715</v>
+      </c>
       <c r="J45" t="s">
         <v>15</v>
       </c>
@@ -3120,6 +3296,10 @@
       <c r="H46">
         <v>79420.600000000006</v>
       </c>
+      <c r="I46">
+        <f t="shared" si="6"/>
+        <v>3054.6384615384618</v>
+      </c>
       <c r="J46" t="s">
         <v>21</v>
       </c>
@@ -3161,6 +3341,10 @@
       <c r="H47">
         <v>77243.100000000006</v>
       </c>
+      <c r="I47">
+        <f t="shared" si="6"/>
+        <v>3089.7240000000002</v>
+      </c>
       <c r="J47" t="s">
         <v>15</v>
       </c>
@@ -3202,6 +3386,10 @@
       <c r="H48">
         <v>72527.199999999997</v>
       </c>
+      <c r="I48">
+        <f t="shared" si="6"/>
+        <v>3453.6761904761902</v>
+      </c>
       <c r="J48" t="s">
         <v>18</v>
       </c>
@@ -3243,6 +3431,10 @@
       <c r="H49">
         <v>52699.4</v>
       </c>
+      <c r="I49">
+        <f t="shared" si="6"/>
+        <v>2509.4952380952382</v>
+      </c>
       <c r="J49" t="s">
         <v>57</v>
       </c>
@@ -3284,6 +3476,10 @@
       <c r="H50">
         <v>29102.3</v>
       </c>
+      <c r="I50">
+        <f t="shared" si="6"/>
+        <v>2078.735714285714</v>
+      </c>
       <c r="J50" t="s">
         <v>15</v>
       </c>
@@ -3325,6 +3521,10 @@
       <c r="H51">
         <v>22282</v>
       </c>
+      <c r="I51">
+        <f t="shared" si="6"/>
+        <v>1714</v>
+      </c>
       <c r="J51" t="s">
         <v>48</v>
       </c>
@@ -3366,6 +3566,10 @@
       <c r="H52">
         <v>20223.900000000001</v>
       </c>
+      <c r="I52">
+        <f t="shared" si="6"/>
+        <v>1685.325</v>
+      </c>
       <c r="J52" t="s">
         <v>15</v>
       </c>
@@ -3406,6 +3610,10 @@
       </c>
       <c r="H53">
         <v>22188.5</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="6"/>
+        <v>1849.0416666666667</v>
       </c>
       <c r="J53" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
computed for covered? column and new car id
</commit_message>
<xml_diff>
--- a/excel/car_database/car database.xlsx
+++ b/excel/car_database/car database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\mikedevs\data-journey\excel\car_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4924FA7D-2C83-4092-BD94-9125C30DC026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E169016F-73D3-4AF7-B6F8-9843BB747E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{196D0D68-09E0-4E97-9B35-E2D7744763AB}"/>
   </bookViews>
@@ -1229,7 +1229,7 @@
   <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1239,6 +1239,7 @@
     <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -1329,6 +1330,14 @@
       <c r="L2">
         <v>50000</v>
       </c>
+      <c r="M2" t="str">
+        <f>IF(H2&lt;=L2,"Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="N2" t="str">
+        <f>CONCATENATE(B2,F2,D2,UPPER(LEFT(J2,3)),RIGHT(A2,3))</f>
+        <v>FD06MTGBLA001</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1374,6 +1383,14 @@
       <c r="L3">
         <v>50000</v>
       </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M53" si="7">IF(H3&lt;=L3,"Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N53" si="8">CONCATENATE(B3,F3,D3,UPPER(LEFT(J3,3)),RIGHT(A3,3))</f>
+        <v>FD06MTGWHI002</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1419,6 +1436,14 @@
       <c r="L4">
         <v>50000</v>
       </c>
+      <c r="M4" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="8"/>
+        <v>FD08MTGGRE003</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1464,6 +1489,14 @@
       <c r="L5">
         <v>50000</v>
       </c>
+      <c r="M5" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="8"/>
+        <v>FD08MTGBLA004</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -1509,6 +1542,14 @@
       <c r="L6">
         <v>50000</v>
       </c>
+      <c r="M6" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="8"/>
+        <v>FD08MTGWHI005</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1554,6 +1595,14 @@
       <c r="L7">
         <v>75000</v>
       </c>
+      <c r="M7" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="8"/>
+        <v>FD06FCSGRE006</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1599,6 +1648,14 @@
       <c r="L8">
         <v>75000</v>
       </c>
+      <c r="M8" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="8"/>
+        <v>FD06FCSGRE007</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1644,6 +1701,14 @@
       <c r="L9">
         <v>75000</v>
       </c>
+      <c r="M9" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="8"/>
+        <v>FD09FCSBLA008</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1689,6 +1754,14 @@
       <c r="L10">
         <v>75000</v>
       </c>
+      <c r="M10" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="8"/>
+        <v>FD13FCSBLA009</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1734,6 +1807,14 @@
       <c r="L11">
         <v>75000</v>
       </c>
+      <c r="M11" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="8"/>
+        <v>FD13FCSWHI010</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1779,6 +1860,14 @@
       <c r="L12">
         <v>75000</v>
       </c>
+      <c r="M12" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="8"/>
+        <v>FD12FCSWHI011</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1824,6 +1913,14 @@
       <c r="L13">
         <v>75000</v>
       </c>
+      <c r="M13" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="8"/>
+        <v>FD13FCSBLA012</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1869,6 +1966,14 @@
       <c r="L14">
         <v>75000</v>
       </c>
+      <c r="M14" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="8"/>
+        <v>FD13FCSBLA013</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1914,6 +2019,14 @@
       <c r="L15">
         <v>100000</v>
       </c>
+      <c r="M15" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="8"/>
+        <v>GM09CMRWHI014</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -1959,8 +2072,16 @@
       <c r="L16">
         <v>100000</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M16" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="8"/>
+        <v>GM12CMRBLA015</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -2004,8 +2125,16 @@
       <c r="L17">
         <v>100000</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M17" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="8"/>
+        <v>GM14CMRWHI016</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -2049,8 +2178,16 @@
       <c r="L18">
         <v>100000</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M18" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="8"/>
+        <v>GM10SLVBLA017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -2094,8 +2231,16 @@
       <c r="L19">
         <v>100000</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M19" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="8"/>
+        <v>GM98SLVBLA018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2139,8 +2284,16 @@
       <c r="L20">
         <v>100000</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M20" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="8"/>
+        <v>GM00SLVBLU019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2184,8 +2337,16 @@
       <c r="L21">
         <v>100000</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M21" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="8"/>
+        <v>TY96CAMGRE020</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2229,8 +2390,16 @@
       <c r="L22">
         <v>100000</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M22" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="8"/>
+        <v>TY98CAMBLA021</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2274,8 +2443,16 @@
       <c r="L23">
         <v>100000</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M23" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="8"/>
+        <v>TY00CAMGRE022</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2319,8 +2496,16 @@
       <c r="L24">
         <v>100000</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M24" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="8"/>
+        <v>TY02CAMBLA023</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -2364,8 +2549,16 @@
       <c r="L25">
         <v>100000</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M25" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="8"/>
+        <v>TY09CAMWHI024</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2409,8 +2602,16 @@
       <c r="L26">
         <v>100000</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M26" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="8"/>
+        <v>TY02CORRED025</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -2454,8 +2655,16 @@
       <c r="L27">
         <v>100000</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M27" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="8"/>
+        <v>TY03CORBLA026</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -2499,8 +2708,16 @@
       <c r="L28">
         <v>100000</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M28" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="8"/>
+        <v>TY14CORBLU027</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -2544,8 +2761,16 @@
       <c r="L29">
         <v>100000</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M29" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="8"/>
+        <v>TY12CORBLA028</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -2589,8 +2814,16 @@
       <c r="L30">
         <v>100000</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M30" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="8"/>
+        <v>TY12CAMBLU029</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -2634,8 +2867,16 @@
       <c r="L31">
         <v>75000</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M31" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="8"/>
+        <v>HO99CIVWHI030</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -2679,8 +2920,16 @@
       <c r="L32">
         <v>75000</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M32" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="8"/>
+        <v>HO01CIVBLU031</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -2724,8 +2973,16 @@
       <c r="L33">
         <v>75000</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M33" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="8"/>
+        <v>HO10CIVBLU032</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -2769,8 +3026,16 @@
       <c r="L34">
         <v>75000</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M34" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="8"/>
+        <v>HO10CIVBLA033</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2814,8 +3079,16 @@
       <c r="L35">
         <v>75000</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M35" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="8"/>
+        <v>HO11CIVBLA034</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -2859,8 +3132,16 @@
       <c r="L36">
         <v>75000</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M36" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="8"/>
+        <v>HO12CIVBLA035</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -2904,8 +3185,16 @@
       <c r="L37">
         <v>75000</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M37" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="8"/>
+        <v>HO13CIVBLA036</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>121</v>
       </c>
@@ -2949,8 +3238,16 @@
       <c r="L38">
         <v>100000</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M38" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N38" t="str">
+        <f t="shared" si="8"/>
+        <v>HO05ODYWHI037</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -2994,8 +3291,16 @@
       <c r="L39">
         <v>100000</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M39" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N39" t="str">
+        <f t="shared" si="8"/>
+        <v>HO07ODYBLA038</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -3039,8 +3344,16 @@
       <c r="L40">
         <v>100000</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M40" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N40" t="str">
+        <f t="shared" si="8"/>
+        <v>HO08ODYWHI039</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -3084,8 +3397,16 @@
       <c r="L41">
         <v>100000</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M41" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N41" t="str">
+        <f t="shared" si="8"/>
+        <v>HO01ODYBLA040</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -3129,8 +3450,16 @@
       <c r="L42">
         <v>100000</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M42" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N42" t="str">
+        <f t="shared" si="8"/>
+        <v>HO14ODYBLA041</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>73</v>
       </c>
@@ -3174,8 +3503,16 @@
       <c r="L43">
         <v>75000</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M43" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" si="8"/>
+        <v>CR04PTCBLU042</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -3219,8 +3556,16 @@
       <c r="L44">
         <v>75000</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M44" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N44" t="str">
+        <f t="shared" si="8"/>
+        <v>CR07PTCGRE043</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -3264,8 +3609,16 @@
       <c r="L45">
         <v>75000</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M45" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N45" t="str">
+        <f t="shared" si="8"/>
+        <v>CR11PTCBLA044</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -3309,8 +3662,16 @@
       <c r="L46">
         <v>75000</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M46" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="N46" t="str">
+        <f t="shared" si="8"/>
+        <v>CR99CARGRE045</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -3354,8 +3715,16 @@
       <c r="L47">
         <v>75000</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M47" t="str">
+        <f t="shared" si="7"/>
+        <v>N</v>
+      </c>
+      <c r="N47" t="str">
+        <f t="shared" si="8"/>
+        <v>CR00CARBLA046</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -3399,8 +3768,16 @@
       <c r="L48">
         <v>75000</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M48" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N48" t="str">
+        <f t="shared" si="8"/>
+        <v>CR04CARWHI047</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -3444,8 +3821,16 @@
       <c r="L49">
         <v>75000</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M49" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N49" t="str">
+        <f t="shared" si="8"/>
+        <v>CR04CARRED048</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>80</v>
       </c>
@@ -3489,8 +3874,16 @@
       <c r="L50">
         <v>100000</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M50" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N50" t="str">
+        <f t="shared" si="8"/>
+        <v>HY11ELABLA049</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>81</v>
       </c>
@@ -3534,8 +3927,16 @@
       <c r="L51">
         <v>100000</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M51" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N51" t="str">
+        <f t="shared" si="8"/>
+        <v>HY12ELABLU050</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>82</v>
       </c>
@@ -3579,8 +3980,16 @@
       <c r="L52">
         <v>100000</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M52" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N52" t="str">
+        <f t="shared" si="8"/>
+        <v>HY13ELABLA051</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>83</v>
       </c>
@@ -3624,8 +4033,16 @@
       <c r="L53">
         <v>100000</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M53" t="str">
+        <f t="shared" si="7"/>
+        <v>Y</v>
+      </c>
+      <c r="N53" t="str">
+        <f t="shared" si="8"/>
+        <v>HY13ELABLU052</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>95</v>
       </c>
@@ -3639,7 +4056,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>84</v>
       </c>
@@ -3653,7 +4070,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>89</v>
       </c>
@@ -3667,7 +4084,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>94</v>
       </c>
@@ -3681,7 +4098,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>92</v>
       </c>
@@ -3695,7 +4112,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>93</v>
       </c>
@@ -3709,7 +4126,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D62" t="s">
         <v>97</v>
       </c>
@@ -3717,7 +4134,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D63" t="s">
         <v>117</v>
       </c>
@@ -3725,7 +4142,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D64" t="s">
         <v>103</v>
       </c>

</xml_diff>